<commit_message>
bf: update ssth form
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Burkina Faso/bf_202301_sch_impact_assessment_1_sites.xlsx
+++ b/SCH-STH/Impact assessments/Burkina Faso/bf_202301_sch_impact_assessment_1_sites.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\WHO\dsa-forms\SCH-STH\Impact assessments\Burkina Faso\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0405A126-1B25-4BEA-9984-6066DD25B788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12255" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="290">
   <si>
     <t>type</t>
   </si>
@@ -369,9 +375,6 @@
     <t>Karangasso-vigue</t>
   </si>
   <si>
-    <t>NDorola</t>
-  </si>
-  <si>
     <t>N'Dorola</t>
   </si>
   <si>
@@ -546,12 +549,6 @@
     <t>TIARAKO</t>
   </si>
   <si>
-    <t>FOFARA</t>
-  </si>
-  <si>
-    <t>N'GORLANI</t>
-  </si>
-  <si>
     <t>KOKORO</t>
   </si>
   <si>
@@ -561,12 +558,6 @@
     <t>SADINA</t>
   </si>
   <si>
-    <t>MOROLABA</t>
-  </si>
-  <si>
-    <t>TEMETEMESSO</t>
-  </si>
-  <si>
     <t>FADONA</t>
   </si>
   <si>
@@ -885,26 +876,32 @@
     <t>default_language</t>
   </si>
   <si>
-    <t>(BF - Jan 2023) impact schisto - 1. Formulaire Village V2.1</t>
-  </si>
-  <si>
-    <t>bf_202301_sch_impact_assessment_1_sites_v2_1</t>
-  </si>
-  <si>
     <t>French</t>
+  </si>
+  <si>
+    <t>Fara</t>
+  </si>
+  <si>
+    <t>Foulasso</t>
+  </si>
+  <si>
+    <t>Kodona</t>
+  </si>
+  <si>
+    <t>Seguedougou</t>
+  </si>
+  <si>
+    <t>(BF - Jan 2023) impact schisto - 1. Formulaire Village V3</t>
+  </si>
+  <si>
+    <t>bf_202301_sch_impact_assessment_1_sites_v3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="28">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -969,152 +966,8 @@
       <name val="Arial"/>
       <charset val="134"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1139,188 +992,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1330,271 +1003,29 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.14996795556505"/>
+        <color theme="0" tint="-0.14993743705557422"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.14996795556505"/>
+        <color theme="0" tint="-0.14993743705557422"/>
       </right>
       <top style="thin">
-        <color theme="0" tint="-0.14996795556505"/>
+        <color theme="0" tint="-0.14993743705557422"/>
       </top>
       <bottom style="thin">
-        <color theme="0" tint="-0.14996795556505"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="0" tint="-0.14993743705557422"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1618,10 +1049,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1630,62 +1057,264 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1701,6 +1330,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1958,37 +1590,36 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5037037037037" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="26.5037037037037" customWidth="1"/>
-    <col min="2" max="2" width="24.4" customWidth="1"/>
-    <col min="3" max="3" width="50.4" customWidth="1"/>
-    <col min="4" max="4" width="23.5037037037037" customWidth="1"/>
-    <col min="5" max="5" width="13.5037037037037" customWidth="1"/>
-    <col min="6" max="6" width="18.5037037037037" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="24.375" customWidth="1"/>
+    <col min="3" max="3" width="50.375" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="30.5037037037037" customWidth="1"/>
-    <col min="11" max="11" width="35.4" customWidth="1"/>
-    <col min="13" max="13" width="17.5037037037037" customWidth="1"/>
+    <col min="8" max="8" width="30.5" customWidth="1"/>
+    <col min="11" max="11" width="35.375" customWidth="1"/>
+    <col min="13" max="13" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="36" spans="1:13">
+    <row r="1" spans="1:13" ht="37.5">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -2025,207 +1656,198 @@
       <c r="L1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="M1" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="12" t="s">
+      <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12" t="s">
+      <c r="J2" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="13" t="s">
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13" t="s">
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="16" t="s">
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" ht="31.5">
       <c r="A5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13" t="s">
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
       <c r="M5" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13" t="s">
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="17"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="15"/>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13" t="s">
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="17"/>
-    </row>
-    <row r="8" ht="42.75" spans="1:13">
-      <c r="A8" s="14" t="s">
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="15"/>
+    </row>
+    <row r="8" spans="1:13" ht="47.25">
+      <c r="A8" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="8" t="s">
         <v>34</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13" t="s">
+      <c r="E8" s="8"/>
+      <c r="F8" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13" t="s">
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
       <c r="M8" s="8"/>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13" t="s">
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13" t="s">
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
       <c r="M9" s="8"/>
     </row>
-    <row r="10" ht="28.5" spans="1:13">
-      <c r="A10" s="14" t="s">
+    <row r="10" spans="1:13" ht="31.5">
+      <c r="A10" s="12" t="s">
         <v>38</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -2234,399 +1856,387 @@
       <c r="C10" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13" t="s">
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="18" t="s">
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="16" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" ht="18.3" customHeight="1" spans="1:13">
-      <c r="A11" s="13" t="s">
+    <row r="11" spans="1:13" ht="18.399999999999999" customHeight="1">
+      <c r="A11" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13" t="s">
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="18"/>
-    </row>
-    <row r="12" ht="18.3" customHeight="1" spans="1:13">
-      <c r="A12" s="13" t="s">
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="16"/>
+    </row>
+    <row r="12" spans="1:13" ht="18.399999999999999" customHeight="1">
+      <c r="A12" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13" t="s">
+      <c r="I12" s="8"/>
+      <c r="J12" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="18"/>
-    </row>
-    <row r="13" ht="18.3" customHeight="1" spans="1:13">
-      <c r="A13" s="13" t="s">
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="16"/>
+    </row>
+    <row r="13" spans="1:13" ht="18.399999999999999" customHeight="1">
+      <c r="A13" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13" t="s">
+      <c r="I13" s="8"/>
+      <c r="J13" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="18"/>
-    </row>
-    <row r="14" ht="18.3" customHeight="1" spans="1:13">
-      <c r="A14" s="13" t="s">
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="16"/>
+    </row>
+    <row r="14" spans="1:13" ht="18.399999999999999" customHeight="1">
+      <c r="A14" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13" t="s">
+      <c r="I14" s="8"/>
+      <c r="J14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="18"/>
-    </row>
-    <row r="15" ht="18.3" customHeight="1" spans="1:13">
-      <c r="A15" s="13" t="s">
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="16"/>
+    </row>
+    <row r="15" spans="1:13" ht="18.399999999999999" customHeight="1">
+      <c r="A15" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13" t="s">
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="18"/>
-    </row>
-    <row r="16" ht="18.3" customHeight="1" spans="1:13">
-      <c r="A16" s="13" t="s">
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="16"/>
+    </row>
+    <row r="16" spans="1:13" ht="18.399999999999999" customHeight="1">
+      <c r="A16" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13" t="s">
+      <c r="I16" s="8"/>
+      <c r="J16" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="18"/>
-    </row>
-    <row r="17" ht="37.8" customHeight="1" spans="1:13">
-      <c r="A17" s="13" t="s">
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="16"/>
+    </row>
+    <row r="17" spans="1:13" ht="37.9" customHeight="1">
+      <c r="A17" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13" t="s">
+      <c r="I17" s="8"/>
+      <c r="J17" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="18"/>
-    </row>
-    <row r="18" ht="37.8" customHeight="1" spans="1:13">
-      <c r="A18" s="13" t="s">
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="16"/>
+    </row>
+    <row r="18" spans="1:13" ht="37.9" customHeight="1">
+      <c r="A18" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13" t="s">
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="18"/>
-    </row>
-    <row r="19" ht="37.8" customHeight="1" spans="1:13">
-      <c r="A19" s="13" t="s">
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="16"/>
+    </row>
+    <row r="19" spans="1:13" ht="37.9" customHeight="1">
+      <c r="A19" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
-      <c r="H19" s="13" t="s">
+      <c r="H19" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13" t="s">
+      <c r="I19" s="8"/>
+      <c r="J19" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="18"/>
-    </row>
-    <row r="20" ht="23.7" customHeight="1" spans="1:13">
-      <c r="A20" s="13" t="s">
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="16"/>
+    </row>
+    <row r="20" spans="1:13" ht="23.65" customHeight="1">
+      <c r="A20" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13" t="s">
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="18"/>
-    </row>
-    <row r="21" ht="36.9" customHeight="1" spans="1:13">
-      <c r="A21" s="13" t="s">
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="16"/>
+    </row>
+    <row r="21" spans="1:13" ht="36.950000000000003" customHeight="1">
+      <c r="A21" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13" t="s">
+      <c r="I21" s="8"/>
+      <c r="J21" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="18"/>
-    </row>
-    <row r="22" ht="36.9" customHeight="1" spans="1:13">
-      <c r="A22" s="13" t="s">
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="16"/>
+    </row>
+    <row r="22" spans="1:13" ht="36.950000000000003" customHeight="1">
+      <c r="A22" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13" t="s">
+      <c r="I22" s="8"/>
+      <c r="J22" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="18"/>
-    </row>
-    <row r="23" ht="28.5" spans="1:13">
-      <c r="A23" s="13" t="s">
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="16"/>
+    </row>
+    <row r="23" spans="1:13" ht="31.5">
+      <c r="A23" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13" t="s">
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="18"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="16"/>
     </row>
     <row r="24" spans="1:13">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13" t="s">
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="18"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="16"/>
     </row>
     <row r="25" spans="1:13">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="18"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="16"/>
     </row>
     <row r="26" spans="1:13">
-      <c r="A26" s="12" t="s">
+      <c r="A26" t="s">
         <v>90</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" t="s">
         <v>91</v>
       </c>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="J26" s="8"/>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27" s="8" t="s">
         <v>92</v>
       </c>
@@ -2637,31 +2247,28 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G145"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B122" activePane="bottomRight" state="frozen"/>
-      <selection/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A134" sqref="$A134:$XFD137"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11:XFD92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5037037037037" defaultRowHeight="14.25" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="16.4" customWidth="1"/>
-    <col min="2" max="2" width="34.1111111111111" customWidth="1"/>
-    <col min="3" max="3" width="14.6" customWidth="1"/>
+    <col min="1" max="1" width="16.375" customWidth="1"/>
+    <col min="2" max="2" width="34.125" customWidth="1"/>
+    <col min="3" max="3" width="14.625" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="16.6962962962963" customWidth="1"/>
+    <col min="7" max="7" width="16.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2687,7 +2294,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -2698,7 +2305,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -2709,7 +2316,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>99</v>
       </c>
@@ -2720,7 +2327,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -2731,7 +2338,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>99</v>
       </c>
@@ -2742,7 +2349,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>99</v>
       </c>
@@ -2753,7 +2360,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>99</v>
       </c>
@@ -2764,7 +2371,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>99</v>
       </c>
@@ -2775,8 +2382,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" s="3" customFormat="1"/>
-    <row r="11" spans="1:3">
+    <row r="10" spans="1:7" s="3" customFormat="1"/>
+    <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
         <v>95</v>
       </c>
@@ -2817,10 +2424,10 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" s="3" customFormat="1" spans="1:1">
+    <row r="14" spans="1:7" s="3" customFormat="1">
       <c r="A14" s="6"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
         <v>96</v>
       </c>
@@ -2834,7 +2441,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
         <v>96</v>
       </c>
@@ -2848,7 +2455,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:7">
       <c r="A17" s="1" t="s">
         <v>96</v>
       </c>
@@ -2862,7 +2469,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:7">
       <c r="A18" s="1" t="s">
         <v>96</v>
       </c>
@@ -2876,7 +2483,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:7">
       <c r="A19" s="1" t="s">
         <v>96</v>
       </c>
@@ -2890,7 +2497,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:7">
       <c r="A20" s="1" t="s">
         <v>96</v>
       </c>
@@ -2898,27 +2505,27 @@
         <v>116</v>
       </c>
       <c r="C20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:7">
       <c r="A21" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" t="s">
         <v>118</v>
-      </c>
-      <c r="C21" t="s">
-        <v>119</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="22" s="3" customFormat="1" spans="1:1">
+    <row r="22" spans="1:7" s="3" customFormat="1">
       <c r="A22" s="6"/>
     </row>
     <row r="23" spans="1:7">
@@ -2926,10 +2533,10 @@
         <v>97</v>
       </c>
       <c r="B23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E23" t="s">
         <v>111</v>
@@ -2942,10 +2549,10 @@
         <v>97</v>
       </c>
       <c r="B24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E24" t="s">
         <v>111</v>
@@ -2958,10 +2565,10 @@
         <v>97</v>
       </c>
       <c r="B25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E25" t="s">
         <v>111</v>
@@ -2974,10 +2581,10 @@
         <v>97</v>
       </c>
       <c r="B26" t="s">
+        <v>122</v>
+      </c>
+      <c r="C26" t="s">
         <v>123</v>
-      </c>
-      <c r="C26" t="s">
-        <v>124</v>
       </c>
       <c r="E26" t="s">
         <v>111</v>
@@ -2990,10 +2597,10 @@
         <v>97</v>
       </c>
       <c r="B27" t="s">
+        <v>124</v>
+      </c>
+      <c r="C27" t="s">
         <v>125</v>
-      </c>
-      <c r="C27" t="s">
-        <v>126</v>
       </c>
       <c r="E27" t="s">
         <v>111</v>
@@ -3006,10 +2613,10 @@
         <v>97</v>
       </c>
       <c r="B28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E28" t="s">
         <v>111</v>
@@ -3022,10 +2629,10 @@
         <v>97</v>
       </c>
       <c r="B29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E29" t="s">
         <v>111</v>
@@ -3038,10 +2645,10 @@
         <v>97</v>
       </c>
       <c r="B30" t="s">
+        <v>128</v>
+      </c>
+      <c r="C30" t="s">
         <v>129</v>
-      </c>
-      <c r="C30" t="s">
-        <v>130</v>
       </c>
       <c r="E30" t="s">
         <v>111</v>
@@ -3054,10 +2661,10 @@
         <v>97</v>
       </c>
       <c r="B31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E31" t="s">
         <v>111</v>
@@ -3070,10 +2677,10 @@
         <v>97</v>
       </c>
       <c r="B32" t="s">
+        <v>131</v>
+      </c>
+      <c r="C32" t="s">
         <v>132</v>
-      </c>
-      <c r="C32" t="s">
-        <v>133</v>
       </c>
       <c r="E32" t="s">
         <v>111</v>
@@ -3086,10 +2693,10 @@
         <v>97</v>
       </c>
       <c r="B33" t="s">
+        <v>133</v>
+      </c>
+      <c r="C33" t="s">
         <v>134</v>
-      </c>
-      <c r="C33" t="s">
-        <v>135</v>
       </c>
       <c r="E33" t="s">
         <v>112</v>
@@ -3102,10 +2709,10 @@
         <v>97</v>
       </c>
       <c r="B34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E34" t="s">
         <v>112</v>
@@ -3118,10 +2725,10 @@
         <v>97</v>
       </c>
       <c r="B35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E35" t="s">
         <v>112</v>
@@ -3134,10 +2741,10 @@
         <v>97</v>
       </c>
       <c r="B36" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C36" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E36" t="s">
         <v>112</v>
@@ -3150,10 +2757,10 @@
         <v>97</v>
       </c>
       <c r="B37" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C37" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E37" t="s">
         <v>112</v>
@@ -3166,10 +2773,10 @@
         <v>97</v>
       </c>
       <c r="B38" t="s">
+        <v>139</v>
+      </c>
+      <c r="C38" t="s">
         <v>140</v>
-      </c>
-      <c r="C38" t="s">
-        <v>141</v>
       </c>
       <c r="E38" t="s">
         <v>112</v>
@@ -3182,10 +2789,10 @@
         <v>97</v>
       </c>
       <c r="B39" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C39" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E39" t="s">
         <v>112</v>
@@ -3198,10 +2805,10 @@
         <v>97</v>
       </c>
       <c r="B40" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C40" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E40" t="s">
         <v>112</v>
@@ -3214,10 +2821,10 @@
         <v>97</v>
       </c>
       <c r="B41" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C41" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E41" t="s">
         <v>112</v>
@@ -3230,10 +2837,10 @@
         <v>97</v>
       </c>
       <c r="B42" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C42" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E42" t="s">
         <v>112</v>
@@ -3246,10 +2853,10 @@
         <v>97</v>
       </c>
       <c r="B43" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C43" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E43" t="s">
         <v>113</v>
@@ -3262,10 +2869,10 @@
         <v>97</v>
       </c>
       <c r="B44" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C44" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E44" t="s">
         <v>113</v>
@@ -3278,10 +2885,10 @@
         <v>97</v>
       </c>
       <c r="B45" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C45" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E45" t="s">
         <v>113</v>
@@ -3294,10 +2901,10 @@
         <v>97</v>
       </c>
       <c r="B46" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C46" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E46" t="s">
         <v>113</v>
@@ -3310,10 +2917,10 @@
         <v>97</v>
       </c>
       <c r="B47" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C47" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E47" t="s">
         <v>113</v>
@@ -3326,10 +2933,10 @@
         <v>97</v>
       </c>
       <c r="B48" t="s">
+        <v>150</v>
+      </c>
+      <c r="C48" t="s">
         <v>151</v>
-      </c>
-      <c r="C48" t="s">
-        <v>152</v>
       </c>
       <c r="E48" t="s">
         <v>113</v>
@@ -3342,10 +2949,10 @@
         <v>97</v>
       </c>
       <c r="B49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E49" t="s">
         <v>113</v>
@@ -3358,10 +2965,10 @@
         <v>97</v>
       </c>
       <c r="B50" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C50" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E50" t="s">
         <v>113</v>
@@ -3374,10 +2981,10 @@
         <v>97</v>
       </c>
       <c r="B51" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C51" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E51" t="s">
         <v>113</v>
@@ -3390,10 +2997,10 @@
         <v>97</v>
       </c>
       <c r="B52" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C52" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E52" t="s">
         <v>113</v>
@@ -3406,10 +3013,10 @@
         <v>97</v>
       </c>
       <c r="B53" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C53" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E53" t="s">
         <v>115</v>
@@ -3422,10 +3029,10 @@
         <v>97</v>
       </c>
       <c r="B54" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C54" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E54" t="s">
         <v>115</v>
@@ -3438,10 +3045,10 @@
         <v>97</v>
       </c>
       <c r="B55" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C55" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E55" t="s">
         <v>115</v>
@@ -3454,10 +3061,10 @@
         <v>97</v>
       </c>
       <c r="B56" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C56" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E56" t="s">
         <v>115</v>
@@ -3470,10 +3077,10 @@
         <v>97</v>
       </c>
       <c r="B57" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C57" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E57" t="s">
         <v>115</v>
@@ -3486,10 +3093,10 @@
         <v>97</v>
       </c>
       <c r="B58" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C58" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E58" t="s">
         <v>115</v>
@@ -3502,10 +3109,10 @@
         <v>97</v>
       </c>
       <c r="B59" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C59" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E59" t="s">
         <v>115</v>
@@ -3518,10 +3125,10 @@
         <v>97</v>
       </c>
       <c r="B60" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C60" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E60" t="s">
         <v>115</v>
@@ -3534,10 +3141,10 @@
         <v>97</v>
       </c>
       <c r="B61" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C61" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E61" t="s">
         <v>115</v>
@@ -3550,10 +3157,10 @@
         <v>97</v>
       </c>
       <c r="B62" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C62" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E62" t="s">
         <v>115</v>
@@ -3566,10 +3173,10 @@
         <v>97</v>
       </c>
       <c r="B63" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C63" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E63" t="s">
         <v>114</v>
@@ -3582,10 +3189,10 @@
         <v>97</v>
       </c>
       <c r="B64" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C64" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E64" t="s">
         <v>114</v>
@@ -3598,10 +3205,10 @@
         <v>97</v>
       </c>
       <c r="B65" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C65" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E65" t="s">
         <v>114</v>
@@ -3614,10 +3221,10 @@
         <v>97</v>
       </c>
       <c r="B66" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C66" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E66" t="s">
         <v>114</v>
@@ -3630,10 +3237,10 @@
         <v>97</v>
       </c>
       <c r="B67" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C67" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E67" t="s">
         <v>114</v>
@@ -3646,10 +3253,10 @@
         <v>97</v>
       </c>
       <c r="B68" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C68" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E68" t="s">
         <v>114</v>
@@ -3662,10 +3269,10 @@
         <v>97</v>
       </c>
       <c r="B69" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C69" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E69" t="s">
         <v>114</v>
@@ -3678,10 +3285,10 @@
         <v>97</v>
       </c>
       <c r="B70" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C70" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E70" t="s">
         <v>114</v>
@@ -3694,10 +3301,10 @@
         <v>97</v>
       </c>
       <c r="B71" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C71" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E71" t="s">
         <v>114</v>
@@ -3710,10 +3317,10 @@
         <v>97</v>
       </c>
       <c r="B72" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C72" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E72" t="s">
         <v>114</v>
@@ -3726,13 +3333,13 @@
         <v>97</v>
       </c>
       <c r="B73" t="s">
-        <v>175</v>
+        <v>284</v>
       </c>
       <c r="C73" t="s">
-        <v>175</v>
+        <v>284</v>
       </c>
       <c r="E73" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F73" s="7"/>
       <c r="G73" s="7"/>
@@ -3742,13 +3349,13 @@
         <v>97</v>
       </c>
       <c r="B74" t="s">
-        <v>176</v>
+        <v>285</v>
       </c>
       <c r="C74" t="s">
-        <v>176</v>
+        <v>285</v>
       </c>
       <c r="E74" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F74" s="7"/>
       <c r="G74" s="7"/>
@@ -3758,13 +3365,13 @@
         <v>97</v>
       </c>
       <c r="B75" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C75" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E75" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F75" s="7"/>
       <c r="G75" s="7"/>
@@ -3774,13 +3381,13 @@
         <v>97</v>
       </c>
       <c r="B76" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C76" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E76" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
@@ -3790,13 +3397,13 @@
         <v>97</v>
       </c>
       <c r="B77" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C77" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E77" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F77" s="7"/>
       <c r="G77" s="7"/>
@@ -3806,13 +3413,13 @@
         <v>97</v>
       </c>
       <c r="B78" t="s">
-        <v>180</v>
+        <v>286</v>
       </c>
       <c r="C78" t="s">
-        <v>180</v>
+        <v>286</v>
       </c>
       <c r="E78" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F78" s="7"/>
       <c r="G78" s="7"/>
@@ -3822,13 +3429,13 @@
         <v>97</v>
       </c>
       <c r="B79" t="s">
-        <v>181</v>
+        <v>287</v>
       </c>
       <c r="C79" t="s">
-        <v>181</v>
+        <v>287</v>
       </c>
       <c r="E79" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F79" s="7"/>
       <c r="G79" s="7"/>
@@ -3838,13 +3445,13 @@
         <v>97</v>
       </c>
       <c r="B80" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C80" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E80" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F80" s="7"/>
       <c r="G80" s="7"/>
@@ -3854,13 +3461,13 @@
         <v>97</v>
       </c>
       <c r="B81" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C81" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E81" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F81" s="7"/>
       <c r="G81" s="7"/>
@@ -3870,13 +3477,13 @@
         <v>97</v>
       </c>
       <c r="B82" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C82" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E82" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F82" s="7"/>
       <c r="G82" s="7"/>
@@ -3886,13 +3493,13 @@
         <v>97</v>
       </c>
       <c r="B83" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C83" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E83" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F83" s="7"/>
       <c r="G83" s="7"/>
@@ -3902,13 +3509,13 @@
         <v>97</v>
       </c>
       <c r="B84" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C84" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="E84" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F84" s="7"/>
       <c r="G84" s="7"/>
@@ -3918,13 +3525,13 @@
         <v>97</v>
       </c>
       <c r="B85" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C85" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E85" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F85" s="7"/>
       <c r="G85" s="7"/>
@@ -3934,13 +3541,13 @@
         <v>97</v>
       </c>
       <c r="B86" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C86" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E86" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F86" s="7"/>
       <c r="G86" s="7"/>
@@ -3950,13 +3557,13 @@
         <v>97</v>
       </c>
       <c r="B87" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C87" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E87" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F87" s="7"/>
       <c r="G87" s="7"/>
@@ -3966,13 +3573,13 @@
         <v>97</v>
       </c>
       <c r="B88" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C88" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="E88" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F88" s="7"/>
       <c r="G88" s="7"/>
@@ -3982,13 +3589,13 @@
         <v>97</v>
       </c>
       <c r="B89" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C89" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E89" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F89" s="7"/>
       <c r="G89" s="7"/>
@@ -3998,13 +3605,13 @@
         <v>97</v>
       </c>
       <c r="B90" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C90" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E90" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F90" s="7"/>
       <c r="G90" s="7"/>
@@ -4014,13 +3621,13 @@
         <v>97</v>
       </c>
       <c r="B91" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C91" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E91" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F91" s="7"/>
       <c r="G91" s="7"/>
@@ -4030,636 +3637,632 @@
         <v>97</v>
       </c>
       <c r="B92" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C92" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="E92" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F92" s="7"/>
       <c r="G92" s="7"/>
     </row>
-    <row r="93" s="3" customFormat="1" spans="1:1">
+    <row r="93" spans="1:7" s="3" customFormat="1">
       <c r="A93" s="6"/>
     </row>
-    <row r="94" ht="15.75" customHeight="1" spans="1:3">
+    <row r="94" spans="1:7" ht="15.75" customHeight="1">
       <c r="A94" t="s">
+        <v>190</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C94" s="8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="A95" t="s">
+        <v>190</v>
+      </c>
+      <c r="B95" t="s">
+        <v>192</v>
+      </c>
+      <c r="C95" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" s="3" customFormat="1">
+      <c r="A96" s="6"/>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97" t="s">
+        <v>193</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C97" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="B94" s="8" t="s">
+    </row>
+    <row r="98" spans="1:7">
+      <c r="A98" t="s">
+        <v>193</v>
+      </c>
+      <c r="B98" t="s">
         <v>196</v>
       </c>
-      <c r="C94" s="8" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3">
-      <c r="A95" t="s">
-        <v>195</v>
-      </c>
-      <c r="B95" t="s">
+      <c r="C98" t="s">
         <v>197</v>
       </c>
-      <c r="C95" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="96" s="3" customFormat="1" spans="1:1">
-      <c r="A96" s="6"/>
-    </row>
-    <row r="97" spans="1:3">
-      <c r="A97" t="s">
-        <v>198</v>
-      </c>
-      <c r="B97" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="C97" s="8" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3">
-      <c r="A98" t="s">
-        <v>198</v>
-      </c>
-      <c r="B98" t="s">
-        <v>201</v>
-      </c>
-      <c r="C98" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="99" s="3" customFormat="1"/>
+    </row>
+    <row r="99" spans="1:7" s="3" customFormat="1"/>
     <row r="100" spans="1:7">
       <c r="A100" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B100" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C100" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="G100" s="7"/>
     </row>
     <row r="101" spans="1:7">
       <c r="A101" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B101" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C101" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="G101" s="7"/>
     </row>
     <row r="102" spans="1:7">
       <c r="A102" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B102" t="s">
         <v>203</v>
       </c>
-      <c r="B102" t="s">
-        <v>208</v>
-      </c>
       <c r="C102" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="G102" s="7"/>
     </row>
     <row r="103" spans="1:7">
       <c r="A103" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B103" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C103" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="G103" s="7"/>
     </row>
     <row r="104" spans="1:7">
       <c r="A104" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="G104" s="7"/>
     </row>
     <row r="105" spans="1:7">
       <c r="A105" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B105" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C105" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G105" s="7"/>
     </row>
     <row r="106" spans="1:7">
       <c r="A106" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B106" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C106" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="G106" s="7"/>
     </row>
     <row r="107" spans="1:7">
       <c r="A107" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B107" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C107" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="G107" s="7"/>
     </row>
     <row r="108" spans="1:7">
       <c r="A108" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B108" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="C108" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="G108" s="7"/>
     </row>
     <row r="109" spans="1:7">
       <c r="A109" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B109" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C109" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="G109" s="7"/>
     </row>
     <row r="110" spans="1:7">
       <c r="A110" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B110" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C110" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G110" s="7"/>
     </row>
     <row r="111" spans="1:7">
       <c r="A111" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B111" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="C111" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="G111" s="7"/>
     </row>
-    <row r="112" s="3" customFormat="1" spans="1:1">
+    <row r="112" spans="1:7" s="3" customFormat="1">
       <c r="A112" s="6"/>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B114" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C114" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B115" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C115" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="116" s="3" customFormat="1" spans="1:1">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" s="3" customFormat="1">
       <c r="A116" s="6"/>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C118" s="9" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B119" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="B119" s="9" t="s">
-        <v>237</v>
-      </c>
       <c r="C119" s="9" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="C120" s="9" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="121" s="3" customFormat="1" spans="1:1">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" s="3" customFormat="1">
       <c r="A121" s="6"/>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B122" s="9" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="C122" s="9" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C123" s="9" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B124" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="B124" s="9" t="s">
-        <v>246</v>
-      </c>
       <c r="C124" s="9" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="C126" s="9" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="127" s="3" customFormat="1" spans="1:1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" s="3" customFormat="1">
       <c r="A127" s="6"/>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C128" s="9" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C129" s="9" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
+        <v>247</v>
+      </c>
+      <c r="B130" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="B130" s="9" t="s">
-        <v>257</v>
-      </c>
       <c r="C130" s="9" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="C131" s="9" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C132" s="9" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="133" s="3" customFormat="1" spans="1:1">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" s="3" customFormat="1">
       <c r="A133" s="6"/>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B134" s="10" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C134" s="10" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B135" s="10" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C135" s="10" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
+        <v>258</v>
+      </c>
+      <c r="B136" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="C136" s="10" t="s">
         <v>263</v>
-      </c>
-      <c r="B136" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="C136" s="10" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B137" s="10" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C137" s="10" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B138" s="10" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C138" s="10" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="139" s="3" customFormat="1" spans="1:1">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" s="3" customFormat="1">
       <c r="A139" s="6"/>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B140" s="10" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C140" s="10" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B141" s="10" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C141" s="10" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B142" s="10" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C142" s="10" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
+        <v>268</v>
+      </c>
+      <c r="B143" s="10" t="s">
         <v>273</v>
       </c>
-      <c r="B143" s="10" t="s">
-        <v>278</v>
-      </c>
       <c r="C143" s="10" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B144" s="10" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="C144" s="10" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B145" s="10" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="C145" s="10" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G1">
-    <extLst/>
-  </autoFilter>
-  <sortState ref="A42:G56">
+  <autoFilter ref="A1:G1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A42:G56">
     <sortCondition ref="B42:B56"/>
   </sortState>
   <conditionalFormatting sqref="E109">
-    <cfRule type="duplicateValues" dxfId="0" priority="81"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="81"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C111">
-    <cfRule type="duplicateValues" dxfId="0" priority="15"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G115">
-    <cfRule type="duplicateValues" dxfId="0" priority="30"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B116">
-    <cfRule type="duplicateValues" dxfId="0" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F119">
-    <cfRule type="duplicateValues" dxfId="0" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B121">
-    <cfRule type="duplicateValues" dxfId="0" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F122">
-    <cfRule type="duplicateValues" dxfId="0" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E124">
-    <cfRule type="duplicateValues" dxfId="0" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B127">
-    <cfRule type="duplicateValues" dxfId="0" priority="7"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G128">
-    <cfRule type="duplicateValues" dxfId="0" priority="25"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B133">
-    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B139">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B100:B112">
-    <cfRule type="duplicateValues" dxfId="0" priority="96"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="97"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="96"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="97"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C100:C110">
-    <cfRule type="duplicateValues" dxfId="0" priority="102"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="103"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="102"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="103"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G124:G125">
-    <cfRule type="duplicateValues" dxfId="0" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G115 G122:G126 G117:G120">
     <cfRule type="duplicateValues" dxfId="0" priority="95"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5037037037037" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="49.2222222222222" customWidth="1"/>
-    <col min="2" max="2" width="42.6666666666667" customWidth="1"/>
+    <col min="1" max="1" width="49.25" customWidth="1"/>
+    <col min="2" max="2" width="47.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="C1" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4673,11 +4276,10 @@
         <v>16</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>